<commit_message>
Formula trimming and extra bracket printing outputs
Deleted a lot of old results text files in preparation for re-creating
them under new protocols. Trimmed all of the formulas. Added extra
diagnostic outputs to printed brackets. Some minor code re-works.
</commit_message>
<xml_diff>
--- a/NCAABB Project/Misc/Formulas Consolidated.xlsx
+++ b/NCAABB Project/Misc/Formulas Consolidated.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="54">
   <si>
     <t>FG%</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>Average 2015(1)</t>
-  </si>
-  <si>
-    <t>Average 2016(1)</t>
-  </si>
-  <si>
-    <t>Average 2016(3)</t>
   </si>
 </sst>
 </file>
@@ -230,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,12 +252,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,12 +560,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AC47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,40 +761,40 @@
         <v>10000</v>
       </c>
       <c r="C3" s="3">
-        <v>-1.337083</v>
+        <v>-1.3</v>
       </c>
       <c r="D3" s="3">
-        <v>-12.297309</v>
+        <v>-12</v>
       </c>
       <c r="E3" s="3">
-        <v>1.6080429999999999</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
-        <v>10.634143</v>
+        <v>10.6</v>
       </c>
       <c r="G3" s="3">
-        <v>12.31531</v>
+        <v>12</v>
       </c>
       <c r="H3" s="3">
-        <v>7.0482579999999997</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3">
-        <v>13.381866</v>
+        <v>13.4</v>
       </c>
       <c r="J3" s="3">
-        <v>6.8533720000000002</v>
+        <v>6.8</v>
       </c>
       <c r="K3" s="3">
-        <v>-9.5051439999999996</v>
+        <v>-9.5</v>
       </c>
       <c r="L3" s="3">
-        <v>15.456194</v>
+        <v>15.5</v>
       </c>
       <c r="M3" s="3">
-        <v>-12.141937</v>
+        <v>-12.1</v>
       </c>
       <c r="N3" s="3">
-        <v>13.525092000000001</v>
+        <v>13.5</v>
       </c>
       <c r="O3" s="3">
         <v>0</v>
@@ -951,40 +939,40 @@
         <v>10000</v>
       </c>
       <c r="C5" s="3">
-        <v>-0.81792337000000004</v>
+        <v>-0.82</v>
       </c>
       <c r="D5" s="3">
-        <v>1.87528926</v>
+        <v>1.88</v>
       </c>
       <c r="E5" s="3">
-        <v>3.87770963</v>
+        <v>3.9</v>
       </c>
       <c r="F5" s="3">
-        <v>5.7408710100000002</v>
+        <v>5.7</v>
       </c>
       <c r="G5" s="3">
-        <v>-3.2913035700000002</v>
+        <v>-3.3</v>
       </c>
       <c r="H5" s="3">
-        <v>-1.84229468</v>
+        <v>-1.8</v>
       </c>
       <c r="I5" s="3">
-        <v>4.5564967300000001</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J5" s="3">
-        <v>1.0755980300000001</v>
+        <v>1</v>
       </c>
       <c r="K5" s="3">
-        <v>-2.0704286399999998</v>
+        <v>-2.1</v>
       </c>
       <c r="L5" s="3">
-        <v>2.7278320000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="M5" s="3">
-        <v>3.8637700599999998</v>
+        <v>3.9</v>
       </c>
       <c r="N5" s="3">
-        <v>2.7973937499999999</v>
+        <v>2.8</v>
       </c>
       <c r="O5" s="3">
         <v>0</v>
@@ -1129,40 +1117,40 @@
         <v>1000</v>
       </c>
       <c r="C7" s="3">
-        <v>-1.4355872999999999</v>
+        <v>-1.4356</v>
       </c>
       <c r="D7" s="3">
-        <v>1.174553</v>
+        <v>1.175</v>
       </c>
       <c r="E7" s="3">
-        <v>-0.3186505</v>
+        <v>-0.31859999999999999</v>
       </c>
       <c r="F7" s="3">
-        <v>-2.0694545</v>
+        <v>-2.0693999999999999</v>
       </c>
       <c r="G7" s="3">
-        <v>-0.80814620000000004</v>
+        <v>-0.80820000000000003</v>
       </c>
       <c r="H7" s="3">
-        <v>5.1496392999999996</v>
+        <v>5.1496000000000004</v>
       </c>
       <c r="I7" s="3">
-        <v>-8.0884126999999992</v>
+        <v>-8.0884</v>
       </c>
       <c r="J7" s="3">
-        <v>3.1297044000000001</v>
+        <v>3.13</v>
       </c>
       <c r="K7" s="3">
-        <v>6.1520308000000004</v>
+        <v>6.1520000000000001</v>
       </c>
       <c r="L7" s="3">
-        <v>10.0600618</v>
+        <v>10.0601</v>
       </c>
       <c r="M7" s="3">
-        <v>3.5383396999999999</v>
+        <v>3.5379999999999998</v>
       </c>
       <c r="N7" s="3">
-        <v>-7.1743825000000001</v>
+        <v>-7.1744000000000003</v>
       </c>
       <c r="O7" s="3">
         <v>0</v>
@@ -1218,40 +1206,40 @@
         <v>1000</v>
       </c>
       <c r="C8" s="3">
-        <v>7.2813929999999996</v>
+        <v>7.3</v>
       </c>
       <c r="D8" s="3">
-        <v>-6.980683</v>
+        <v>-7</v>
       </c>
       <c r="E8" s="3">
-        <v>-7.3539279999999998</v>
+        <v>-7.3</v>
       </c>
       <c r="F8" s="3">
-        <v>4.0162250000000004</v>
+        <v>4</v>
       </c>
       <c r="G8" s="3">
-        <v>-4.1949829999999997</v>
+        <v>-4</v>
       </c>
       <c r="H8" s="3">
-        <v>11.409782999999999</v>
+        <v>11</v>
       </c>
       <c r="I8" s="3">
-        <v>1.9178269999999999</v>
+        <v>1.9</v>
       </c>
       <c r="J8" s="3">
-        <v>8.1681760000000008</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K8" s="3">
-        <v>11.830549</v>
+        <v>11.8</v>
       </c>
       <c r="L8" s="3">
-        <v>37.225538</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="M8" s="3">
-        <v>8.0987290000000005</v>
+        <v>8</v>
       </c>
       <c r="N8" s="3">
-        <v>-2.4736760000000002</v>
+        <v>-2.5</v>
       </c>
       <c r="O8" s="3">
         <v>0</v>
@@ -1275,28 +1263,28 @@
         <v>0</v>
       </c>
       <c r="V8" s="3">
-        <v>16.917126</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="W8" s="3">
-        <v>33.229607000000001</v>
+        <v>33</v>
       </c>
       <c r="X8" s="3">
-        <v>22.993276000000002</v>
+        <v>23</v>
       </c>
       <c r="Y8" s="3">
-        <v>15.950146</v>
+        <v>16</v>
       </c>
       <c r="Z8" s="3">
-        <v>-1.2839970000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA8" s="3">
-        <v>-6.5804790000000004</v>
+        <v>-7</v>
       </c>
       <c r="AB8" s="3">
-        <v>-16.465807999999999</v>
+        <v>-16.5</v>
       </c>
       <c r="AC8" s="3">
-        <v>6.6766740000000002</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -1307,40 +1295,40 @@
         <v>10000</v>
       </c>
       <c r="C9" s="2">
-        <v>1.6018698</v>
+        <v>1.6020000000000001</v>
       </c>
       <c r="D9" s="3">
-        <v>-1.4856902000000001</v>
+        <v>-1.486</v>
       </c>
       <c r="E9" s="3">
-        <v>-4.3682800000000001E-2</v>
+        <v>-4.3700000000000003E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>-1.5707792</v>
+        <v>-1.5708</v>
       </c>
       <c r="G9" s="3">
-        <v>2.4437281999999998</v>
+        <v>2.4437000000000002</v>
       </c>
       <c r="H9" s="3">
-        <v>2.2706905000000002</v>
+        <v>2.2707000000000002</v>
       </c>
       <c r="I9" s="3">
-        <v>5.9098004</v>
+        <v>5.9</v>
       </c>
       <c r="J9" s="3">
-        <v>3.0189493000000001</v>
+        <v>3.0188999999999999</v>
       </c>
       <c r="K9" s="3">
-        <v>1.2125967</v>
+        <v>1.2130000000000001</v>
       </c>
       <c r="L9" s="3">
-        <v>10.9239804</v>
+        <v>10.92</v>
       </c>
       <c r="M9" s="3">
-        <v>0.9288362</v>
+        <v>0.92879999999999996</v>
       </c>
       <c r="N9" s="3">
-        <v>1.0214649</v>
+        <v>1.0215000000000001</v>
       </c>
       <c r="O9" s="3">
         <v>0</v>
@@ -1396,40 +1384,40 @@
         <v>1000</v>
       </c>
       <c r="C10" s="2">
-        <v>-1.9644545600000001</v>
+        <v>-1.96</v>
       </c>
       <c r="D10" s="3">
-        <v>3.4147865099999999</v>
+        <v>3.42</v>
       </c>
       <c r="E10" s="3">
-        <v>-2.5354507900000001</v>
+        <v>-2.54</v>
       </c>
       <c r="F10" s="3">
-        <v>3.8111727800000001</v>
+        <v>3.81</v>
       </c>
       <c r="G10" s="3">
-        <v>0.30633146999999999</v>
+        <v>0.31</v>
       </c>
       <c r="H10" s="3">
-        <v>-3.5018665499999999</v>
+        <v>-3.5</v>
       </c>
       <c r="I10" s="3">
-        <v>1.24163435</v>
+        <v>1.24</v>
       </c>
       <c r="J10" s="3">
-        <v>-1.0257912199999999</v>
+        <v>-1.03</v>
       </c>
       <c r="K10" s="3">
-        <v>2.6028296599999998</v>
+        <v>3</v>
       </c>
       <c r="L10" s="3">
-        <v>3.2938255600000002</v>
+        <v>3.29</v>
       </c>
       <c r="M10" s="3">
-        <v>0.88182415000000003</v>
+        <v>0.88</v>
       </c>
       <c r="N10" s="3">
-        <v>-6.02276948</v>
+        <v>-6.02</v>
       </c>
       <c r="O10" s="3">
         <v>0</v>
@@ -1485,61 +1473,61 @@
         <v>1000</v>
       </c>
       <c r="C11" s="2">
-        <v>8.4100111200000001</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
-        <v>7.4347651199999998</v>
+        <v>7.4</v>
       </c>
       <c r="E11" s="3">
-        <v>2.6282800100000001</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3">
-        <v>25.176360979999998</v>
+        <v>25</v>
       </c>
       <c r="G11" s="3">
-        <v>4.6819255999999996</v>
+        <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>-12.59749313</v>
+        <v>-13</v>
       </c>
       <c r="I11" s="3">
-        <v>11.3274469</v>
+        <v>11</v>
       </c>
       <c r="J11" s="3">
-        <v>6.9722966700000004</v>
+        <v>7</v>
       </c>
       <c r="K11" s="3">
-        <v>2.3286335399999998</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L11" s="3">
-        <v>12.14731473</v>
+        <v>12.1</v>
       </c>
       <c r="M11" s="3">
-        <v>-7.7230094300000003</v>
+        <v>-8</v>
       </c>
       <c r="N11" s="3">
-        <v>0.92731105999999996</v>
+        <v>0.9</v>
       </c>
       <c r="O11" s="3">
-        <v>10.8546145</v>
+        <v>11</v>
       </c>
       <c r="P11" s="3">
-        <v>-14.049847059999999</v>
+        <v>-14</v>
       </c>
       <c r="Q11" s="3">
-        <v>0.94457869000000005</v>
+        <v>0.9</v>
       </c>
       <c r="R11" s="3">
-        <v>1.67739715</v>
+        <v>2</v>
       </c>
       <c r="S11" s="3">
-        <v>3.1224196900000001</v>
+        <v>3</v>
       </c>
       <c r="T11" s="3">
-        <v>-5.3682316300000004</v>
+        <v>-5.4</v>
       </c>
       <c r="U11" s="3">
-        <v>0.47485442</v>
+        <v>0.5</v>
       </c>
       <c r="V11" s="3">
         <v>0</v>
@@ -1574,40 +1562,40 @@
         <v>10000</v>
       </c>
       <c r="C12" s="2">
-        <v>9.6776319500000003</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D12" s="3">
-        <v>-10.46280672</v>
+        <v>-10.46</v>
       </c>
       <c r="E12" s="3">
-        <v>-8.1746880799999992</v>
+        <v>-8.18</v>
       </c>
       <c r="F12" s="3">
-        <v>10.915090770000001</v>
+        <v>10.91</v>
       </c>
       <c r="G12" s="3">
-        <v>-4.6816467499999996</v>
+        <v>-4.68</v>
       </c>
       <c r="H12" s="3">
-        <v>7.3022278800000002</v>
+        <v>7.3</v>
       </c>
       <c r="I12" s="3">
-        <v>8.4891603399999997</v>
+        <v>8.5</v>
       </c>
       <c r="J12" s="3">
-        <v>-2.16935046</v>
+        <v>-2.17</v>
       </c>
       <c r="K12" s="3">
-        <v>-7.7197698099999998</v>
+        <v>-8</v>
       </c>
       <c r="L12" s="3">
-        <v>14.305133720000001</v>
+        <v>14.3</v>
       </c>
       <c r="M12" s="3">
-        <v>10.20286231</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="N12" s="3">
-        <v>-13.924560749999999</v>
+        <v>-13.93</v>
       </c>
       <c r="O12" s="3">
         <v>0</v>
@@ -1663,61 +1651,61 @@
         <v>10000</v>
       </c>
       <c r="C13" s="2">
-        <v>16.064940929999999</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="D13" s="3">
-        <v>-8.7361942900000003</v>
+        <v>-8.6999999999999993</v>
       </c>
       <c r="E13" s="3">
-        <v>-4.6565062900000003</v>
+        <v>-4.7</v>
       </c>
       <c r="F13" s="3">
-        <v>26.817722969999998</v>
+        <v>27</v>
       </c>
       <c r="G13" s="3">
-        <v>-12.74577921</v>
+        <v>-12.8</v>
       </c>
       <c r="H13" s="3">
-        <v>-10.294611250000001</v>
+        <v>-10.3</v>
       </c>
       <c r="I13" s="3">
-        <v>9.2700749800000004</v>
+        <v>9</v>
       </c>
       <c r="J13" s="3">
-        <v>-18.645357090000001</v>
+        <v>-18.600000000000001</v>
       </c>
       <c r="K13" s="3">
-        <v>-33.16469231</v>
+        <v>-33.200000000000003</v>
       </c>
       <c r="L13" s="3">
-        <v>16.231784699999999</v>
+        <v>16</v>
       </c>
       <c r="M13" s="3">
-        <v>26.852242839999999</v>
+        <v>26.9</v>
       </c>
       <c r="N13" s="3">
-        <v>-21.68083201</v>
+        <v>-22</v>
       </c>
       <c r="O13" s="3">
-        <v>-22.736397929999999</v>
+        <v>-23</v>
       </c>
       <c r="P13" s="3">
-        <v>-9.7312913999999999</v>
+        <v>-10</v>
       </c>
       <c r="Q13" s="3">
-        <v>1.6925418400000001</v>
+        <v>1.7</v>
       </c>
       <c r="R13" s="3">
-        <v>15.92944977</v>
+        <v>16</v>
       </c>
       <c r="S13" s="3">
-        <v>2.1763587100000001</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="T13" s="3">
-        <v>10.076594829999999</v>
+        <v>10.1</v>
       </c>
       <c r="U13" s="3">
-        <v>34.409825499999997</v>
+        <v>34</v>
       </c>
       <c r="V13" s="3">
         <v>0</v>
@@ -1841,40 +1829,40 @@
         <v>13</v>
       </c>
       <c r="C15" s="3">
-        <v>-1.0775031850000001</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="D15" s="3">
-        <v>-5.2110098699999998</v>
+        <v>-5.0999999999999996</v>
       </c>
       <c r="E15" s="3">
-        <v>2.7428763150000002</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <v>8.1875070050000005</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G15" s="3">
-        <v>4.512003215</v>
+        <v>4.3</v>
       </c>
       <c r="H15" s="3">
-        <v>2.6029816600000002</v>
+        <v>3</v>
       </c>
       <c r="I15" s="3">
-        <v>8.9691813650000007</v>
+        <v>9</v>
       </c>
       <c r="J15" s="3">
-        <v>3.9644850150000002</v>
+        <v>4</v>
       </c>
       <c r="K15" s="3">
-        <v>-5.7877863200000004</v>
+        <v>-6</v>
       </c>
       <c r="L15" s="3">
-        <v>7.7417361600000003</v>
+        <v>7.76</v>
       </c>
       <c r="M15" s="3">
-        <v>-4.1390834700000001</v>
+        <v>-4</v>
       </c>
       <c r="N15" s="3">
-        <v>8.1612428749999992</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="O15" s="3">
         <v>0</v>
@@ -1930,40 +1918,40 @@
         <v>13</v>
       </c>
       <c r="C16" s="3">
-        <v>2.0833333333333299</v>
+        <v>2.1</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <v>2.3333333333333335</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F16" s="3">
-        <v>1.6666666666666667</v>
+        <v>1.7</v>
       </c>
       <c r="G16" s="3">
-        <v>1.1666666666666667</v>
+        <v>1.2</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
       </c>
       <c r="I16" s="3">
-        <v>3.3333333333333335</v>
+        <v>3.3</v>
       </c>
       <c r="J16" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.3</v>
       </c>
       <c r="K16" s="3">
         <v>1</v>
       </c>
       <c r="L16" s="3">
-        <v>1.6666666666666667</v>
+        <v>1.7</v>
       </c>
       <c r="M16" s="3">
-        <v>1.3333333333333333</v>
+        <v>1.3</v>
       </c>
       <c r="N16" s="3">
-        <v>4.666666666666667</v>
+        <v>4.7</v>
       </c>
       <c r="O16" s="3">
         <v>0</v>
@@ -2019,40 +2007,40 @@
         <v>13</v>
       </c>
       <c r="C17" s="3">
-        <v>-1.1968645600000001</v>
+        <v>-1.2</v>
       </c>
       <c r="D17" s="3">
-        <v>-3.0824889099999999</v>
+        <v>-2.9816669999999998</v>
       </c>
       <c r="E17" s="3">
-        <v>1.7223673799999999</v>
+        <v>1.8604670000000001</v>
       </c>
       <c r="F17" s="3">
-        <v>4.7685198399999997</v>
+        <v>4.7435330000000002</v>
       </c>
       <c r="G17" s="3">
-        <v>2.73862008</v>
+        <v>2.6</v>
       </c>
       <c r="H17" s="3">
-        <v>3.4518675399999998</v>
+        <v>3.4498669999999998</v>
       </c>
       <c r="I17" s="3">
-        <v>3.28331668</v>
+        <v>3.3038669999999999</v>
       </c>
       <c r="J17" s="3">
-        <v>3.6862248100000001</v>
+        <v>3.6433330000000002</v>
       </c>
       <c r="K17" s="3">
-        <v>-1.8078472800000001</v>
+        <v>-2</v>
       </c>
       <c r="L17" s="3">
-        <v>8.5145113699999992</v>
+        <v>8.5300329999999995</v>
       </c>
       <c r="M17" s="3">
-        <v>-1.5799424099999999</v>
+        <v>-2</v>
       </c>
       <c r="N17" s="3">
-        <v>3.04936775</v>
+        <v>3.0418669999999999</v>
       </c>
       <c r="O17" s="3">
         <v>0</v>
@@ -2108,40 +2096,40 @@
         <v>13</v>
       </c>
       <c r="C18" s="3">
-        <v>-0.49718096750000002</v>
+        <v>-0.5</v>
       </c>
       <c r="D18" s="3">
-        <v>-2.6832892350000002</v>
+        <v>-2.61</v>
       </c>
       <c r="E18" s="3">
-        <v>1.2808548325</v>
+        <v>1.3839999999999999</v>
       </c>
       <c r="F18" s="3">
-        <v>3.1836950774999999</v>
+        <v>3.2</v>
       </c>
       <c r="G18" s="3">
-        <v>2.6648971074999999</v>
+        <v>2.5840000000000001</v>
       </c>
       <c r="H18" s="3">
-        <v>3.1565732799999999</v>
+        <v>3.1549999999999998</v>
       </c>
       <c r="I18" s="3">
-        <v>3.9399376075000001</v>
+        <v>4</v>
       </c>
       <c r="J18" s="3">
-        <v>3.5194059324999998</v>
+        <v>3.4870000000000001</v>
       </c>
       <c r="K18" s="3">
-        <v>-1.0527362849999999</v>
+        <v>-1.06</v>
       </c>
       <c r="L18" s="3">
-        <v>9.1168786300000004</v>
+        <v>9.1270000000000007</v>
       </c>
       <c r="M18" s="3">
-        <v>-0.95274776000000005</v>
+        <v>-0.9</v>
       </c>
       <c r="N18" s="3">
-        <v>2.5423920375</v>
+        <v>2.5369999999999999</v>
       </c>
       <c r="O18" s="3">
         <v>0</v>
@@ -2197,40 +2185,40 @@
         <v>13</v>
       </c>
       <c r="C19" s="3">
-        <v>-0.79063568600000012</v>
+        <v>-0.8</v>
       </c>
       <c r="D19" s="3">
-        <v>-1.4636740860000002</v>
+        <v>-1</v>
       </c>
       <c r="E19" s="3">
-        <v>0.51759370799999993</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
-        <v>3.3091906180000001</v>
+        <v>3</v>
       </c>
       <c r="G19" s="3">
-        <v>2.1931839799999997</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>1.8248853140000001</v>
+        <v>1.8</v>
       </c>
       <c r="I19" s="3">
-        <v>3.4002769560000004</v>
+        <v>3</v>
       </c>
       <c r="J19" s="3">
-        <v>2.6103665019999998</v>
+        <v>2.6</v>
       </c>
       <c r="K19" s="3">
-        <v>-0.32162309599999983</v>
+        <v>0</v>
       </c>
       <c r="L19" s="3">
-        <v>7.9522680160000006</v>
+        <v>8</v>
       </c>
       <c r="M19" s="3">
-        <v>-0.58583337800000002</v>
+        <v>-0.6</v>
       </c>
       <c r="N19" s="3">
-        <v>0.82935973400000029</v>
+        <v>0.8</v>
       </c>
       <c r="O19" s="3">
         <v>0</v>
@@ -2278,160 +2266,159 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B23" s="5">
         <v>2010</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C23" s="4">
         <v>2011</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D23" s="4">
         <v>2012</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E23" s="4">
         <v>2013</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F23" s="4">
         <v>2014</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G23" s="4">
         <v>2015</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H23" s="4">
         <v>2016</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2">
+        <v>118</v>
+      </c>
+      <c r="C24" s="3">
+        <v>75</v>
+      </c>
+      <c r="D24" s="3">
+        <v>57</v>
+      </c>
+      <c r="E24" s="3">
+        <v>69</v>
+      </c>
+      <c r="F24" s="3">
+        <v>52</v>
+      </c>
+      <c r="G24" s="3">
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C25" s="3">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="D25" s="3">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E25" s="3">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="F25" s="3">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="G25" s="3">
-        <v>99</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="2">
-        <v>137</v>
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C26" s="3">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D26" s="3">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="E26" s="3">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="F26" s="3">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G26" s="3">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="3">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D27" s="3">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E27" s="3">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F27" s="3">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G27" s="3">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="3">
-        <v>135</v>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D28" s="3">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="E28" s="3">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F28" s="3">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="G28" s="3">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>13</v>
@@ -2440,21 +2427,21 @@
         <v>13</v>
       </c>
       <c r="D29" s="3">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E29" s="3">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="F29" s="3">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="G29" s="3">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>13</v>
@@ -2463,70 +2450,70 @@
         <v>13</v>
       </c>
       <c r="D30" s="3">
-        <v>164</v>
-      </c>
-      <c r="E30" s="3">
-        <v>50</v>
-      </c>
-      <c r="F30" s="3">
-        <v>29</v>
-      </c>
-      <c r="G30" s="3">
+        <v>172</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="3">
+        <v>161</v>
+      </c>
+      <c r="F31" s="3">
+        <v>40</v>
+      </c>
+      <c r="G31" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="3">
+        <v>134</v>
+      </c>
+      <c r="G32" s="3">
         <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="3">
-        <v>172</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="3">
-        <v>161</v>
-      </c>
-      <c r="F32" s="3">
-        <v>40</v>
-      </c>
-      <c r="G32" s="3">
-        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>13</v>
@@ -2541,7 +2528,7 @@
         <v>13</v>
       </c>
       <c r="F33" s="3">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
@@ -2549,7 +2536,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>13</v>
@@ -2563,16 +2550,16 @@
       <c r="E34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="3">
-        <v>149</v>
+      <c r="F34" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G34" s="3">
-        <v>32</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>13</v>
@@ -2590,35 +2577,38 @@
         <v>13</v>
       </c>
       <c r="G35" s="3">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>13</v>
+      <c r="C36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="2">
+        <v>66</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="3">
-        <v>170</v>
+      <c r="F36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>13</v>
@@ -2627,7 +2617,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="2">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>13</v>
@@ -2644,7 +2634,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
@@ -2652,11 +2642,11 @@
       <c r="C38" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="2">
-        <v>50</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>13</v>
+      <c r="D38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="3">
+        <v>58</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>13</v>
@@ -2670,7 +2660,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>13</v>
@@ -2682,7 +2672,7 @@
         <v>13</v>
       </c>
       <c r="E39" s="3">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>13</v>
@@ -2696,7 +2686,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>13</v>
@@ -2707,11 +2697,11 @@
       <c r="D40" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="3">
-        <v>26</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>13</v>
+      <c r="E40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="6">
+        <v>34</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>13</v>
@@ -2722,7 +2712,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
@@ -2736,11 +2726,11 @@
       <c r="E41" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="6">
-        <v>34</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>13</v>
+      <c r="F41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="6">
+        <v>43</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>13</v>
@@ -2748,56 +2738,56 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="6">
-        <v>43</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="B42" s="2">
+        <v>59</v>
+      </c>
+      <c r="C42" s="3">
+        <v>50</v>
+      </c>
+      <c r="D42" s="3">
+        <v>88</v>
+      </c>
+      <c r="E42" s="3">
+        <v>61</v>
+      </c>
+      <c r="F42" s="3">
+        <v>38</v>
+      </c>
+      <c r="G42" s="3">
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="2">
-        <v>59</v>
-      </c>
-      <c r="C43" s="3">
-        <v>50</v>
-      </c>
-      <c r="D43" s="3">
-        <v>88</v>
-      </c>
-      <c r="E43" s="3">
-        <v>61</v>
-      </c>
-      <c r="F43" s="3">
-        <v>38</v>
-      </c>
-      <c r="G43" s="3">
-        <v>96</v>
+        <v>28</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="6">
+        <v>81</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>13</v>
@@ -2805,71 +2795,68 @@
       <c r="C44" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="6">
+        <v>39</v>
+      </c>
+      <c r="G44" s="3">
         <v>81</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="6">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="B45" s="2">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3">
+        <v>57</v>
+      </c>
+      <c r="D45" s="3">
+        <v>120</v>
+      </c>
+      <c r="E45" s="3">
+        <v>112</v>
+      </c>
+      <c r="F45" s="3">
+        <v>68</v>
       </c>
       <c r="G45" s="3">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="2">
-        <v>62</v>
-      </c>
-      <c r="C46" s="3">
-        <v>57</v>
-      </c>
-      <c r="D46" s="3">
-        <v>120</v>
+        <v>17</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E46" s="3">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="F46" s="3">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G46" s="3">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>13</v>
@@ -2881,41 +2868,18 @@
         <v>13</v>
       </c>
       <c r="E47" s="3">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="F47" s="3">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G47" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="3">
-        <v>133</v>
-      </c>
-      <c r="F48" s="3">
-        <v>72</v>
-      </c>
-      <c r="G48" s="3">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actual Results mode, results text files
Applied a lot of formulas and saved the results. Slight tweak to handle
a variable number of headers when displaying brackets in the GUI. Added
new mode to output the actual results for a tournament given the worths
column in the stats file.
</commit_message>
<xml_diff>
--- a/NCAABB Project/Misc/Formulas Consolidated.xlsx
+++ b/NCAABB Project/Misc/Formulas Consolidated.xlsx
@@ -565,7 +565,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,7 +2384,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F27" s="3">
         <v>38</v>
@@ -2672,7 +2672,7 @@
         <v>13</v>
       </c>
       <c r="E39" s="3">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added support for 2016 Tournament
</commit_message>
<xml_diff>
--- a/NCAABB Project/Misc/Formulas Consolidated.xlsx
+++ b/NCAABB Project/Misc/Formulas Consolidated.xlsx
@@ -313,12 +313,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -630,7 +630,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33:V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,90 +3314,90 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C33" s="3">
-        <f>(C4-$AI4)/($AH4-$AI4)+(C7-$AI7)/($AH7-$AI7)+(C11-$AI11)/($AH11-$AI11)+(C13-$AI13)/($AH13-$AI13)+(C15-$AI15)/($AH15-$AI15)+(C17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" ref="C33:N33" si="1">(C4-$AI4)/($AH4-$AI4)+(C7-$AI7)/($AH7-$AI7)+(C11-$AI11)/($AH11-$AI11)+(C13-$AI13)/($AH13-$AI13)+(C15-$AI15)/($AH15-$AI15)+(C17-$AI17)/($AH17-$AI17)</f>
         <v>2.9149624116193884</v>
       </c>
       <c r="D33" s="3">
-        <f>(D4-$AI4)/($AH4-$AI4)+(D7-$AI7)/($AH7-$AI7)+(D11-$AI11)/($AH11-$AI11)+(D13-$AI13)/($AH13-$AI13)+(D15-$AI15)/($AH15-$AI15)+(D17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>2.0057347758648643</v>
       </c>
       <c r="E33" s="3">
-        <f>(E4-$AI4)/($AH4-$AI4)+(E7-$AI7)/($AH7-$AI7)+(E11-$AI11)/($AH11-$AI11)+(E13-$AI13)/($AH13-$AI13)+(E15-$AI15)/($AH15-$AI15)+(E17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>2.8994191577185897</v>
       </c>
       <c r="F33" s="3">
-        <f>(F4-$AI4)/($AH4-$AI4)+(F7-$AI7)/($AH7-$AI7)+(F11-$AI11)/($AH11-$AI11)+(F13-$AI13)/($AH13-$AI13)+(F15-$AI15)/($AH15-$AI15)+(F17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>3.9967031615819066</v>
       </c>
       <c r="G33" s="3">
-        <f>(G4-$AI4)/($AH4-$AI4)+(G7-$AI7)/($AH7-$AI7)+(G11-$AI11)/($AH11-$AI11)+(G13-$AI13)/($AH13-$AI13)+(G15-$AI15)/($AH15-$AI15)+(G17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>2.3146567276376544</v>
       </c>
       <c r="H33" s="3">
-        <f>(H4-$AI4)/($AH4-$AI4)+(H7-$AI7)/($AH7-$AI7)+(H11-$AI11)/($AH11-$AI11)+(H13-$AI13)/($AH13-$AI13)+(H15-$AI15)/($AH15-$AI15)+(H17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>1.9544895191925802</v>
       </c>
       <c r="I33" s="3">
-        <f>(I4-$AI4)/($AH4-$AI4)+(I7-$AI7)/($AH7-$AI7)+(I11-$AI11)/($AH11-$AI11)+(I13-$AI13)/($AH13-$AI13)+(I15-$AI15)/($AH15-$AI15)+(I17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>3.0147169690774342</v>
       </c>
       <c r="J33" s="3">
-        <f>(J4-$AI4)/($AH4-$AI4)+(J7-$AI7)/($AH7-$AI7)+(J11-$AI11)/($AH11-$AI11)+(J13-$AI13)/($AH13-$AI13)+(J15-$AI15)/($AH15-$AI15)+(J17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>1.9745786748716938</v>
       </c>
       <c r="K33" s="3">
-        <f>(K4-$AI4)/($AH4-$AI4)+(K7-$AI7)/($AH7-$AI7)+(K11-$AI11)/($AH11-$AI11)+(K13-$AI13)/($AH13-$AI13)+(K15-$AI15)/($AH15-$AI15)+(K17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>2.1209781193107764</v>
       </c>
       <c r="L33" s="3">
-        <f>(L4-$AI4)/($AH4-$AI4)+(L7-$AI7)/($AH7-$AI7)+(L11-$AI11)/($AH11-$AI11)+(L13-$AI13)/($AH13-$AI13)+(L15-$AI15)/($AH15-$AI15)+(L17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>3.5195982710551879</v>
       </c>
       <c r="M33" s="3">
-        <f>(M4-$AI4)/($AH4-$AI4)+(M7-$AI7)/($AH7-$AI7)+(M11-$AI11)/($AH11-$AI11)+(M13-$AI13)/($AH13-$AI13)+(M15-$AI15)/($AH15-$AI15)+(M17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>2.6984748724173451</v>
       </c>
       <c r="N33" s="3">
-        <f>(N4-$AI4)/($AH4-$AI4)+(N7-$AI7)/($AH7-$AI7)+(N11-$AI11)/($AH11-$AI11)+(N13-$AI13)/($AH13-$AI13)+(N15-$AI15)/($AH15-$AI15)+(N17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="1"/>
         <v>3.2208941634575958</v>
       </c>
       <c r="P33" s="3">
-        <f>(P4-$AI4)/($AH4-$AI4)+(P7-$AI7)/($AH7-$AI7)+(P11-$AI11)/($AH11-$AI11)+(P13-$AI13)/($AH13-$AI13)+(P15-$AI15)/($AH15-$AI15)+(P17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" ref="P33:V33" si="2">(P4-$AI4)/($AH4-$AI4)+(P7-$AI7)/($AH7-$AI7)+(P11-$AI11)/($AH11-$AI11)+(P13-$AI13)/($AH13-$AI13)+(P15-$AI15)/($AH15-$AI15)+(P17-$AI17)/($AH17-$AI17)</f>
         <v>2.2462317041501882</v>
       </c>
       <c r="Q33" s="3">
-        <f>(Q4-$AI4)/($AH4-$AI4)+(Q7-$AI7)/($AH7-$AI7)+(Q11-$AI11)/($AH11-$AI11)+(Q13-$AI13)/($AH13-$AI13)+(Q15-$AI15)/($AH15-$AI15)+(Q17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>1.8353326029753556</v>
       </c>
       <c r="R33" s="3">
-        <f>(R4-$AI4)/($AH4-$AI4)+(R7-$AI7)/($AH7-$AI7)+(R11-$AI11)/($AH11-$AI11)+(R13-$AI13)/($AH13-$AI13)+(R15-$AI15)/($AH15-$AI15)+(R17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>2.4926588139111434</v>
       </c>
       <c r="S33" s="3">
-        <f>(S4-$AI4)/($AH4-$AI4)+(S7-$AI7)/($AH7-$AI7)+(S11-$AI11)/($AH11-$AI11)+(S13-$AI13)/($AH13-$AI13)+(S15-$AI15)/($AH15-$AI15)+(S17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>3.0445685109626526</v>
       </c>
       <c r="T33" s="3">
-        <f>(T4-$AI4)/($AH4-$AI4)+(T7-$AI7)/($AH7-$AI7)+(T11-$AI11)/($AH11-$AI11)+(T13-$AI13)/($AH13-$AI13)+(T15-$AI15)/($AH15-$AI15)+(T17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>2.2198055332464603</v>
       </c>
       <c r="U33" s="3">
-        <f>(U4-$AI4)/($AH4-$AI4)+(U7-$AI7)/($AH7-$AI7)+(U11-$AI11)/($AH11-$AI11)+(U13-$AI13)/($AH13-$AI13)+(U15-$AI15)/($AH15-$AI15)+(U17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>2.4272617167734816</v>
       </c>
       <c r="V33" s="3">
-        <f>(V4-$AI4)/($AH4-$AI4)+(V7-$AI7)/($AH7-$AI7)+(V11-$AI11)/($AH11-$AI11)+(V13-$AI13)/($AH13-$AI13)+(V15-$AI15)/($AH15-$AI15)+(V17-$AI17)/($AH17-$AI17)</f>
+        <f t="shared" si="2"/>
         <v>3.2765749347482096</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
@@ -3876,7 +3876,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3902,7 +3902,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -3928,7 +3928,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -3954,7 +3954,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -3980,7 +3980,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -4006,7 +4006,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -4032,7 +4032,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -4058,7 +4058,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -4082,7 +4082,7 @@
       <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">

</xml_diff>

<commit_message>
Fixed GUI for 'Select Formula', added outputs on 'Run Formula Batch'
</commit_message>
<xml_diff>
--- a/NCAABB Project/Misc/Formulas Consolidated.xlsx
+++ b/NCAABB Project/Misc/Formulas Consolidated.xlsx
@@ -628,9 +628,9 @@
   <dimension ref="A1:AI71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33:V33"/>
+      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,6 +3447,9 @@
       <c r="G38" s="3">
         <v>99</v>
       </c>
+      <c r="H38" s="3">
+        <v>67</v>
+      </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
@@ -3470,6 +3473,9 @@
       <c r="G39" s="3">
         <v>39</v>
       </c>
+      <c r="H39" s="3">
+        <v>65</v>
+      </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -3493,6 +3499,9 @@
       <c r="G40" s="3">
         <v>36</v>
       </c>
+      <c r="H40" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -3516,6 +3525,9 @@
       <c r="G41" s="3">
         <v>91</v>
       </c>
+      <c r="H41" s="3">
+        <v>59</v>
+      </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
@@ -3539,6 +3551,9 @@
       <c r="G42" s="3">
         <v>61</v>
       </c>
+      <c r="H42" s="3">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -3562,6 +3577,9 @@
       <c r="G43" s="3">
         <v>42</v>
       </c>
+      <c r="H43" s="3">
+        <v>52</v>
+      </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -3585,6 +3603,9 @@
       <c r="G44" s="3">
         <v>86</v>
       </c>
+      <c r="H44" s="3">
+        <v>43</v>
+      </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -3608,6 +3629,9 @@
       <c r="G45" s="3">
         <v>32</v>
       </c>
+      <c r="H45" s="3">
+        <v>38</v>
+      </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -3657,7 +3681,9 @@
       <c r="G47" s="6">
         <v>42</v>
       </c>
-      <c r="H47" s="6"/>
+      <c r="H47" s="6">
+        <v>31</v>
+      </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -3681,6 +3707,9 @@
       <c r="G48" s="3">
         <v>85</v>
       </c>
+      <c r="H48" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -3704,6 +3733,9 @@
       <c r="G49" s="3">
         <v>73</v>
       </c>
+      <c r="H49" s="3">
+        <v>62</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -3727,6 +3759,9 @@
       <c r="G50" s="3">
         <v>32</v>
       </c>
+      <c r="H50" s="3">
+        <v>42</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -3750,6 +3785,9 @@
       <c r="G51" s="3">
         <v>32</v>
       </c>
+      <c r="H51" s="3">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -3773,6 +3811,9 @@
       <c r="G52" s="3">
         <v>167</v>
       </c>
+      <c r="H52" s="3">
+        <v>92</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -3796,6 +3837,9 @@
       <c r="G53" s="3">
         <v>170</v>
       </c>
+      <c r="H53" s="3">
+        <v>38</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -4079,7 +4123,9 @@
       <c r="G64" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H64" s="6"/>
+      <c r="H64" s="6">
+        <v>50</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
@@ -4103,7 +4149,9 @@
       <c r="G65" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="6"/>
+      <c r="H65" s="6">
+        <v>62</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
@@ -4127,6 +4175,9 @@
       <c r="G66" s="3">
         <v>96</v>
       </c>
+      <c r="H66" s="3">
+        <v>49</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
@@ -4176,6 +4227,9 @@
       <c r="G68" s="3">
         <v>81</v>
       </c>
+      <c r="H68" s="3">
+        <v>59</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
@@ -4199,6 +4253,9 @@
       <c r="G69" s="3">
         <v>89</v>
       </c>
+      <c r="H69" s="3">
+        <v>87</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
@@ -4222,6 +4279,9 @@
       <c r="G70" s="3">
         <v>86</v>
       </c>
+      <c r="H70" s="3">
+        <v>89</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
@@ -4244,6 +4304,9 @@
       </c>
       <c r="G71" s="3">
         <v>88</v>
+      </c>
+      <c r="H71" s="3">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>